<commit_message>
Se ha creado el PWDN
</commit_message>
<xml_diff>
--- a/STM32H7/PIN_MAP/STM32H743_pinmap_LQFP144.xlsx
+++ b/STM32H7/PIN_MAP/STM32H743_pinmap_LQFP144.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Desktop\STM32 MCUs\STM32H7\PIN_MAP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\RENBOARD\renBOARD\STM32H7\PIN_MAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394FF8A6-31E7-48ED-A2DB-42F891D7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B7FAB7-8768-4497-8E95-80B2EF9F3538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MCU" sheetId="2" r:id="rId1"/>
@@ -1166,7 +1166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1187,7 +1187,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,18 +1208,19 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
           <color auto="1"/>
-        </right>
+        </left>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1240,19 +1240,18 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
           <color auto="1"/>
-        </left>
-        <right/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1345,9 +1344,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C90ADF66-1734-4F11-9F79-E083103B87F2}" name="PinGroups" displayName="PinGroups" ref="A1:C15" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:C15" xr:uid="{C90ADF66-1734-4F11-9F79-E083103B87F2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{436C5C27-975C-4CC5-9D2A-2C67261D740B}" name="CHECK" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{436C5C27-975C-4CC5-9D2A-2C67261D740B}" name="CHECK" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{EA66865C-D3FF-4851-A8B9-6EE052C64D78}" name="Pin Groups2" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{73AB9FB0-C954-4E44-9582-836A80D86DF5}" name="Descripción" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{73AB9FB0-C954-4E44-9582-836A80D86DF5}" name="Descripción" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1361,6 +1360,11 @@
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="CLOCK"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:F170">
     <sortCondition ref="E31:E177"/>
@@ -1370,8 +1374,8 @@
     <tableColumn id="2" xr3:uid="{1B91728E-4165-4DF1-B2EC-3BAEF4FC6339}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{2FF983DD-E44E-442F-991B-103D9229F29E}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{7D84E1CA-4EEF-4766-A512-36241937E00F}" uniqueName="4" name="Signal" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{0F5E23F6-424B-48C0-AF94-91EB25B7D066}" uniqueName="6" name="Grupo" queryTableFieldId="6" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{D3CE05D1-E853-4CE8-AA28-5044D2BEF4BD}" uniqueName="5" name="Label" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{0F5E23F6-424B-48C0-AF94-91EB25B7D066}" uniqueName="6" name="Grupo" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D3CE05D1-E853-4CE8-AA28-5044D2BEF4BD}" uniqueName="5" name="Label" queryTableFieldId="5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1667,7 +1671,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -2482,7 +2486,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2669,8 +2673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D15C7FF-AFE0-4631-8AE0-A2212C07C97C}">
   <dimension ref="A1:F177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2707,17 +2711,16 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12" t="s">
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2725,17 +2728,16 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2743,17 +2745,16 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2761,17 +2762,16 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12" t="s">
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2779,17 +2779,16 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12" t="s">
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2797,17 +2796,16 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12" t="s">
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2815,17 +2813,16 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12" t="s">
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2833,17 +2830,16 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2851,17 +2847,16 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12" t="s">
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2869,17 +2864,16 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12" t="s">
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2887,17 +2881,16 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" t="s">
         <v>147</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2905,17 +2898,16 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2923,17 +2915,16 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12" t="s">
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2941,17 +2932,16 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" t="s">
         <v>142</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12" t="s">
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2959,57 +2949,56 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" t="s">
         <v>142</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>40</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" t="s">
         <v>179</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
         <v>180</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>41</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
         <v>182</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3017,17 +3006,16 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" t="s">
         <v>154</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12" t="s">
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3035,17 +3023,16 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" t="s">
         <v>155</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12" t="s">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3053,17 +3040,16 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" t="s">
         <v>156</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12" t="s">
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3071,17 +3057,16 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" t="s">
         <v>157</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12" t="s">
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3089,17 +3074,16 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12" t="s">
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3107,77 +3091,76 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" t="s">
         <v>151</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>42</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" t="s">
         <v>183</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="12" t="s">
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
         <v>184</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>43</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" t="s">
         <v>185</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="12" t="s">
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
         <v>186</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" t="s">
         <v>323</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>44</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" t="s">
         <v>187</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="12" t="s">
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
         <v>188</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" t="s">
         <v>323</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3185,19 +3168,19 @@
       <c r="A28">
         <v>29</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" t="s">
         <v>168</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" t="s">
         <v>112</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3205,59 +3188,59 @@
       <c r="A29">
         <v>30</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" t="s">
         <v>169</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
         <v>115</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" t="s">
         <v>112</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>63</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" t="s">
         <v>208</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" t="s">
         <v>209</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" t="s">
         <v>210</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>64</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" t="s">
         <v>211</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" t="s">
         <v>209</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" t="s">
         <v>210</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3265,17 +3248,16 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" t="s">
         <v>170</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12" t="s">
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3283,57 +3265,56 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>65</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" t="s">
         <v>212</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" t="s">
         <v>209</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" t="s">
         <v>210</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>66</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" t="s">
         <v>213</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" t="s">
         <v>209</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" t="s">
         <v>210</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3341,17 +3322,16 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" t="s">
         <v>174</v>
       </c>
-      <c r="C36" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12" t="s">
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3359,17 +3339,16 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12" t="s">
+      <c r="D37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3377,17 +3356,16 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" t="s">
         <v>175</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" t="s">
         <v>142</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12" t="s">
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3395,17 +3373,16 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" t="s">
         <v>176</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" t="s">
         <v>177</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12" t="s">
+      <c r="D39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3413,117 +3390,116 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" t="s">
         <v>178</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" t="s">
         <v>142</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>67</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" t="s">
         <v>214</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" t="s">
         <v>209</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" t="s">
         <v>210</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>68</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" t="s">
         <v>215</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" t="s">
         <v>209</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" t="s">
         <v>210</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>69</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" t="s">
         <v>216</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" t="s">
         <v>209</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" t="s">
         <v>210</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" t="s">
         <v>7</v>
       </c>
-      <c r="F43" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>73</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" t="s">
         <v>218</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" t="s">
         <v>219</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" t="s">
         <v>220</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" t="s">
         <v>7</v>
       </c>
-      <c r="F44" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>74</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" t="s">
         <v>221</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" t="s">
         <v>219</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" t="s">
         <v>220</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3531,17 +3507,16 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" t="s">
         <v>189</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12" t="s">
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3549,17 +3524,16 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12" t="s">
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3567,17 +3541,16 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" t="s">
         <v>191</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12" t="s">
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3585,17 +3558,16 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" t="s">
         <v>142</v>
       </c>
-      <c r="D49" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12" t="s">
+      <c r="D49" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3603,117 +3575,116 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" t="s">
         <v>151</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" t="s">
         <v>142</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>75</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" t="s">
         <v>222</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" t="s">
         <v>219</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" t="s">
         <v>220</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>76</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" t="s">
         <v>223</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" t="s">
         <v>219</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" t="s">
         <v>220</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" t="s">
         <v>7</v>
       </c>
-      <c r="F52" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>77</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" t="s">
         <v>224</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" t="s">
         <v>219</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" t="s">
         <v>220</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" t="s">
         <v>7</v>
       </c>
-      <c r="F53" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>16</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" t="s">
         <v>152</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="12" t="s">
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" t="s">
         <v>17</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" t="s">
         <v>2</v>
       </c>
-      <c r="F54" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>17</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" t="s">
         <v>153</v>
       </c>
-      <c r="C55" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="12" t="s">
+      <c r="C55" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" t="s">
         <v>16</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" t="s">
         <v>2</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3721,17 +3692,16 @@
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" t="s">
         <v>202</v>
       </c>
-      <c r="C56" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12" t="s">
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" t="s">
+        <v>34</v>
+      </c>
+      <c r="F56" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3739,17 +3709,16 @@
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" t="s">
         <v>203</v>
       </c>
-      <c r="C57" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12" t="s">
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3757,17 +3726,16 @@
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" t="s">
         <v>204</v>
       </c>
-      <c r="C58" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12" t="s">
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" t="s">
+        <v>34</v>
+      </c>
+      <c r="F58" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3775,17 +3743,16 @@
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B59" t="s">
         <v>205</v>
       </c>
-      <c r="C59" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12" t="s">
+      <c r="C59" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" t="s">
+        <v>34</v>
+      </c>
+      <c r="F59" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3793,17 +3760,16 @@
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="12" t="s">
+      <c r="B60" t="s">
         <v>206</v>
       </c>
-      <c r="C60" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12" t="s">
+      <c r="C60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" t="s">
+        <v>34</v>
+      </c>
+      <c r="F60" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3811,17 +3777,16 @@
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B61" t="s">
         <v>207</v>
       </c>
-      <c r="C61" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12" t="s">
+      <c r="C61" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" t="s">
+        <v>34</v>
+      </c>
+      <c r="F61" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3829,17 +3794,16 @@
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" t="s">
         <v>150</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" t="s">
         <v>142</v>
       </c>
-      <c r="D62" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12" t="s">
+      <c r="D62" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3847,157 +3811,156 @@
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B63" t="s">
         <v>151</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" t="s">
         <v>142</v>
       </c>
-      <c r="D63" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>164</v>
       </c>
-      <c r="B64" s="12" t="s">
+      <c r="B64" t="s">
         <v>309</v>
       </c>
-      <c r="C64" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D64" s="12" t="s">
+      <c r="C64" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" t="s">
         <v>14</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" t="s">
         <v>2</v>
       </c>
-      <c r="F64" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>165</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B65" t="s">
         <v>310</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D65" s="12" t="s">
+      <c r="C65" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" t="s">
         <v>15</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" t="s">
         <v>2</v>
       </c>
-      <c r="F65" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>50</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B66" t="s">
         <v>192</v>
       </c>
-      <c r="C66" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D66" s="12" t="s">
+      <c r="C66" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" t="s">
         <v>193</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" t="s">
         <v>124</v>
       </c>
-      <c r="F66" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F66" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>51</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B67" t="s">
         <v>194</v>
       </c>
-      <c r="C67" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D67" s="12" t="s">
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" t="s">
         <v>195</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E67" t="s">
         <v>124</v>
       </c>
-      <c r="F67" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>52</v>
       </c>
-      <c r="B68" s="12" t="s">
+      <c r="B68" t="s">
         <v>196</v>
       </c>
-      <c r="C68" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D68" s="12" t="s">
+      <c r="C68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" t="s">
         <v>197</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" t="s">
         <v>124</v>
       </c>
-      <c r="F68" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>53</v>
       </c>
-      <c r="B69" s="12" t="s">
+      <c r="B69" t="s">
         <v>198</v>
       </c>
-      <c r="C69" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D69" s="12" t="s">
+      <c r="C69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" t="s">
         <v>199</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" t="s">
         <v>124</v>
       </c>
-      <c r="F69" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F69" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>54</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B70" t="s">
         <v>200</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D70" s="12" t="s">
+      <c r="C70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" t="s">
         <v>201</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E70" t="s">
         <v>124</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4005,17 +3968,16 @@
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" s="12" t="s">
+      <c r="B71" t="s">
         <v>217</v>
       </c>
-      <c r="C71" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12" t="s">
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" t="s">
+        <v>34</v>
+      </c>
+      <c r="F71" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4023,17 +3985,16 @@
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B72" t="s">
         <v>150</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C72" t="s">
         <v>142</v>
       </c>
-      <c r="D72" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12" t="s">
+      <c r="D72" t="s">
+        <v>34</v>
+      </c>
+      <c r="F72" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4041,117 +4002,116 @@
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" s="12" t="s">
+      <c r="B73" t="s">
         <v>151</v>
       </c>
-      <c r="C73" s="12" t="s">
+      <c r="C73" t="s">
         <v>142</v>
       </c>
-      <c r="D73" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>34</v>
+      </c>
+      <c r="F73" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>24</v>
       </c>
-      <c r="B74" s="12" t="s">
+      <c r="B74" t="s">
         <v>158</v>
       </c>
-      <c r="C74" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D74" s="12" t="s">
+      <c r="C74" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" t="s">
         <v>159</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="E74" t="s">
         <v>1</v>
       </c>
-      <c r="F74" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F74" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>25</v>
       </c>
-      <c r="B75" s="12" t="s">
+      <c r="B75" t="s">
         <v>160</v>
       </c>
-      <c r="C75" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D75" s="12" t="s">
+      <c r="C75" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" t="s">
         <v>161</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" t="s">
         <v>1</v>
       </c>
-      <c r="F75" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F75" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>26</v>
       </c>
-      <c r="B76" s="12" t="s">
+      <c r="B76" t="s">
         <v>162</v>
       </c>
-      <c r="C76" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D76" s="12" t="s">
+      <c r="C76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" t="s">
         <v>163</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E76" t="s">
         <v>1</v>
       </c>
-      <c r="F76" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F76" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>27</v>
       </c>
-      <c r="B77" s="12" t="s">
+      <c r="B77" t="s">
         <v>164</v>
       </c>
-      <c r="C77" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D77" s="12" t="s">
+      <c r="C77" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" t="s">
         <v>165</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" t="s">
         <v>1</v>
       </c>
-      <c r="F77" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F77" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>28</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B78" t="s">
         <v>166</v>
       </c>
-      <c r="C78" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D78" s="12" t="s">
+      <c r="C78" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" t="s">
         <v>167</v>
       </c>
-      <c r="E78" s="12" t="s">
+      <c r="E78" t="s">
         <v>1</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4159,37 +4119,36 @@
       <c r="A79">
         <v>78</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="B79" t="s">
         <v>225</v>
       </c>
-      <c r="C79" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D79" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79" t="s">
+        <v>34</v>
+      </c>
+      <c r="F79" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B80" t="s">
         <v>226</v>
       </c>
-      <c r="C80" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D80" s="12" t="s">
+      <c r="C80" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80" t="s">
         <v>227</v>
       </c>
-      <c r="E80" s="12" t="s">
+      <c r="E80" t="s">
         <v>1</v>
       </c>
-      <c r="F80" s="12" t="s">
+      <c r="F80" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4197,17 +4156,16 @@
       <c r="A81">
         <v>80</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B81" t="s">
         <v>228</v>
       </c>
-      <c r="C81" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12" t="s">
+      <c r="C81" t="s">
+        <v>33</v>
+      </c>
+      <c r="D81" t="s">
+        <v>34</v>
+      </c>
+      <c r="F81" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4215,17 +4173,16 @@
       <c r="A82">
         <v>81</v>
       </c>
-      <c r="B82" s="12" t="s">
+      <c r="B82" t="s">
         <v>229</v>
       </c>
-      <c r="C82" s="12" t="s">
+      <c r="C82" t="s">
         <v>142</v>
       </c>
-      <c r="D82" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12" t="s">
+      <c r="D82" t="s">
+        <v>34</v>
+      </c>
+      <c r="F82" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4233,17 +4190,16 @@
       <c r="A83">
         <v>82</v>
       </c>
-      <c r="B83" s="12" t="s">
+      <c r="B83" t="s">
         <v>151</v>
       </c>
-      <c r="C83" s="12" t="s">
+      <c r="C83" t="s">
         <v>142</v>
       </c>
-      <c r="D83" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12" t="s">
+      <c r="D83" t="s">
+        <v>34</v>
+      </c>
+      <c r="F83" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4251,17 +4207,16 @@
       <c r="A84">
         <v>83</v>
       </c>
-      <c r="B84" s="12" t="s">
+      <c r="B84" t="s">
         <v>230</v>
       </c>
-      <c r="C84" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12" t="s">
+      <c r="C84" t="s">
+        <v>33</v>
+      </c>
+      <c r="D84" t="s">
+        <v>34</v>
+      </c>
+      <c r="F84" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4269,17 +4224,16 @@
       <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B85" t="s">
         <v>231</v>
       </c>
-      <c r="C85" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12" t="s">
+      <c r="C85" t="s">
+        <v>33</v>
+      </c>
+      <c r="D85" t="s">
+        <v>34</v>
+      </c>
+      <c r="F85" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4287,17 +4241,16 @@
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B86" t="s">
         <v>232</v>
       </c>
-      <c r="C86" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12" t="s">
+      <c r="C86" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" t="s">
+        <v>34</v>
+      </c>
+      <c r="F86" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4305,17 +4258,16 @@
       <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B87" t="s">
         <v>233</v>
       </c>
-      <c r="C87" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12" t="s">
+      <c r="C87" t="s">
+        <v>33</v>
+      </c>
+      <c r="D87" t="s">
+        <v>34</v>
+      </c>
+      <c r="F87" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4323,17 +4275,16 @@
       <c r="A88">
         <v>87</v>
       </c>
-      <c r="B88" s="12" t="s">
+      <c r="B88" t="s">
         <v>234</v>
       </c>
-      <c r="C88" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D88" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12" t="s">
+      <c r="C88" t="s">
+        <v>33</v>
+      </c>
+      <c r="D88" t="s">
+        <v>34</v>
+      </c>
+      <c r="F88" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4341,17 +4292,16 @@
       <c r="A89">
         <v>88</v>
       </c>
-      <c r="B89" s="12" t="s">
+      <c r="B89" t="s">
         <v>235</v>
       </c>
-      <c r="C89" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D89" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12" t="s">
+      <c r="C89" t="s">
+        <v>33</v>
+      </c>
+      <c r="D89" t="s">
+        <v>34</v>
+      </c>
+      <c r="F89" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4359,17 +4309,16 @@
       <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90" s="12" t="s">
+      <c r="B90" t="s">
         <v>236</v>
       </c>
-      <c r="C90" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D90" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12" t="s">
+      <c r="C90" t="s">
+        <v>33</v>
+      </c>
+      <c r="D90" t="s">
+        <v>34</v>
+      </c>
+      <c r="F90" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4377,17 +4326,16 @@
       <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91" s="12" t="s">
+      <c r="B91" t="s">
         <v>150</v>
       </c>
-      <c r="C91" s="12" t="s">
+      <c r="C91" t="s">
         <v>142</v>
       </c>
-      <c r="D91" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12" t="s">
+      <c r="D91" t="s">
+        <v>34</v>
+      </c>
+      <c r="F91" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4395,17 +4343,16 @@
       <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92" s="12" t="s">
+      <c r="B92" t="s">
         <v>151</v>
       </c>
-      <c r="C92" s="12" t="s">
+      <c r="C92" t="s">
         <v>142</v>
       </c>
-      <c r="D92" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12" t="s">
+      <c r="D92" t="s">
+        <v>34</v>
+      </c>
+      <c r="F92" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4413,37 +4360,36 @@
       <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93" s="12" t="s">
+      <c r="B93" t="s">
         <v>237</v>
       </c>
-      <c r="C93" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D93" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>33</v>
+      </c>
+      <c r="D93" t="s">
+        <v>34</v>
+      </c>
+      <c r="F93" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>99</v>
       </c>
-      <c r="B94" s="12" t="s">
+      <c r="B94" t="s">
         <v>244</v>
       </c>
-      <c r="C94" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D94" s="12" t="s">
+      <c r="C94" t="s">
+        <v>33</v>
+      </c>
+      <c r="D94" t="s">
         <v>245</v>
       </c>
-      <c r="E94" s="12" t="s">
+      <c r="E94" t="s">
         <v>324</v>
       </c>
-      <c r="F94" s="12" t="s">
+      <c r="F94" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4451,17 +4397,16 @@
       <c r="A95">
         <v>94</v>
       </c>
-      <c r="B95" s="12" t="s">
+      <c r="B95" t="s">
         <v>239</v>
       </c>
-      <c r="C95" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D95" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12" t="s">
+      <c r="C95" t="s">
+        <v>33</v>
+      </c>
+      <c r="D95" t="s">
+        <v>34</v>
+      </c>
+      <c r="F95" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4469,17 +4414,16 @@
       <c r="A96">
         <v>95</v>
       </c>
-      <c r="B96" s="12" t="s">
+      <c r="B96" t="s">
         <v>240</v>
       </c>
-      <c r="C96" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D96" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12" t="s">
+      <c r="C96" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" t="s">
+        <v>34</v>
+      </c>
+      <c r="F96" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4487,17 +4431,16 @@
       <c r="A97">
         <v>96</v>
       </c>
-      <c r="B97" s="12" t="s">
+      <c r="B97" t="s">
         <v>241</v>
       </c>
-      <c r="C97" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D97" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E97" s="12"/>
-      <c r="F97" s="12" t="s">
+      <c r="C97" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" t="s">
+        <v>34</v>
+      </c>
+      <c r="F97" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4505,17 +4448,16 @@
       <c r="A98">
         <v>97</v>
       </c>
-      <c r="B98" s="12" t="s">
+      <c r="B98" t="s">
         <v>242</v>
       </c>
-      <c r="C98" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D98" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12" t="s">
+      <c r="C98" t="s">
+        <v>33</v>
+      </c>
+      <c r="D98" t="s">
+        <v>34</v>
+      </c>
+      <c r="F98" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4523,77 +4465,76 @@
       <c r="A99">
         <v>98</v>
       </c>
-      <c r="B99" s="12" t="s">
+      <c r="B99" t="s">
         <v>243</v>
       </c>
-      <c r="C99" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D99" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>33</v>
+      </c>
+      <c r="D99" t="s">
+        <v>34</v>
+      </c>
+      <c r="F99" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>100</v>
       </c>
-      <c r="B100" s="12" t="s">
+      <c r="B100" t="s">
         <v>246</v>
       </c>
-      <c r="C100" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D100" s="12" t="s">
+      <c r="C100" t="s">
+        <v>33</v>
+      </c>
+      <c r="D100" t="s">
         <v>247</v>
       </c>
-      <c r="E100" s="12" t="s">
+      <c r="E100" t="s">
         <v>324</v>
       </c>
-      <c r="F100" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F100" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>101</v>
       </c>
-      <c r="B101" s="12" t="s">
+      <c r="B101" t="s">
         <v>248</v>
       </c>
-      <c r="C101" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D101" s="12" t="s">
+      <c r="C101" t="s">
+        <v>33</v>
+      </c>
+      <c r="D101" t="s">
         <v>249</v>
       </c>
-      <c r="E101" s="12" t="s">
+      <c r="E101" t="s">
         <v>324</v>
       </c>
-      <c r="F101" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F101" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>169</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B102" t="s">
         <v>315</v>
       </c>
-      <c r="C102" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D102" s="12" t="s">
+      <c r="C102" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102" t="s">
         <v>316</v>
       </c>
-      <c r="E102" s="12" t="s">
+      <c r="E102" t="s">
         <v>324</v>
       </c>
-      <c r="F102" s="12" t="s">
+      <c r="F102" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4601,17 +4542,16 @@
       <c r="A103">
         <v>102</v>
       </c>
-      <c r="B103" s="12" t="s">
+      <c r="B103" t="s">
         <v>150</v>
       </c>
-      <c r="C103" s="12" t="s">
+      <c r="C103" t="s">
         <v>142</v>
       </c>
-      <c r="D103" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E103" s="12"/>
-      <c r="F103" s="12" t="s">
+      <c r="D103" t="s">
+        <v>34</v>
+      </c>
+      <c r="F103" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4619,17 +4559,16 @@
       <c r="A104">
         <v>103</v>
       </c>
-      <c r="B104" s="12" t="s">
+      <c r="B104" t="s">
         <v>151</v>
       </c>
-      <c r="C104" s="12" t="s">
+      <c r="C104" t="s">
         <v>142</v>
       </c>
-      <c r="D104" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12" t="s">
+      <c r="D104" t="s">
+        <v>34</v>
+      </c>
+      <c r="F104" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4637,17 +4576,16 @@
       <c r="A105">
         <v>104</v>
       </c>
-      <c r="B105" s="12" t="s">
+      <c r="B105" t="s">
         <v>250</v>
       </c>
-      <c r="C105" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D105" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E105" s="12"/>
-      <c r="F105" s="12" t="s">
+      <c r="C105" t="s">
+        <v>33</v>
+      </c>
+      <c r="D105" t="s">
+        <v>34</v>
+      </c>
+      <c r="F105" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4655,17 +4593,16 @@
       <c r="A106">
         <v>105</v>
       </c>
-      <c r="B106" s="12" t="s">
+      <c r="B106" t="s">
         <v>251</v>
       </c>
-      <c r="C106" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D106" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E106" s="12"/>
-      <c r="F106" s="12" t="s">
+      <c r="C106" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106" t="s">
+        <v>34</v>
+      </c>
+      <c r="F106" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4673,17 +4610,16 @@
       <c r="A107">
         <v>106</v>
       </c>
-      <c r="B107" s="12" t="s">
+      <c r="B107" t="s">
         <v>252</v>
       </c>
-      <c r="C107" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D107" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12" t="s">
+      <c r="C107" t="s">
+        <v>33</v>
+      </c>
+      <c r="D107" t="s">
+        <v>34</v>
+      </c>
+      <c r="F107" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4691,17 +4627,16 @@
       <c r="A108">
         <v>107</v>
       </c>
-      <c r="B108" s="12" t="s">
+      <c r="B108" t="s">
         <v>253</v>
       </c>
-      <c r="C108" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E108" s="12"/>
-      <c r="F108" s="12" t="s">
+      <c r="C108" t="s">
+        <v>33</v>
+      </c>
+      <c r="D108" t="s">
+        <v>34</v>
+      </c>
+      <c r="F108" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4709,17 +4644,16 @@
       <c r="A109">
         <v>108</v>
       </c>
-      <c r="B109" s="12" t="s">
+      <c r="B109" t="s">
         <v>254</v>
       </c>
-      <c r="C109" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D109" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E109" s="12"/>
-      <c r="F109" s="12" t="s">
+      <c r="C109" t="s">
+        <v>33</v>
+      </c>
+      <c r="D109" t="s">
+        <v>34</v>
+      </c>
+      <c r="F109" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4727,17 +4661,16 @@
       <c r="A110">
         <v>109</v>
       </c>
-      <c r="B110" s="12" t="s">
+      <c r="B110" t="s">
         <v>255</v>
       </c>
-      <c r="C110" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D110" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E110" s="12"/>
-      <c r="F110" s="12" t="s">
+      <c r="C110" t="s">
+        <v>33</v>
+      </c>
+      <c r="D110" t="s">
+        <v>34</v>
+      </c>
+      <c r="F110" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4745,17 +4678,16 @@
       <c r="A111">
         <v>110</v>
       </c>
-      <c r="B111" s="12" t="s">
+      <c r="B111" t="s">
         <v>256</v>
       </c>
-      <c r="C111" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D111" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12" t="s">
+      <c r="C111" t="s">
+        <v>33</v>
+      </c>
+      <c r="D111" t="s">
+        <v>34</v>
+      </c>
+      <c r="F111" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4763,17 +4695,16 @@
       <c r="A112">
         <v>111</v>
       </c>
-      <c r="B112" s="12" t="s">
+      <c r="B112" t="s">
         <v>257</v>
       </c>
-      <c r="C112" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D112" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12" t="s">
+      <c r="C112" t="s">
+        <v>33</v>
+      </c>
+      <c r="D112" t="s">
+        <v>34</v>
+      </c>
+      <c r="F112" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4781,17 +4712,16 @@
       <c r="A113">
         <v>112</v>
       </c>
-      <c r="B113" s="12" t="s">
+      <c r="B113" t="s">
         <v>258</v>
       </c>
-      <c r="C113" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D113" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E113" s="12"/>
-      <c r="F113" s="12" t="s">
+      <c r="C113" t="s">
+        <v>33</v>
+      </c>
+      <c r="D113" t="s">
+        <v>34</v>
+      </c>
+      <c r="F113" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4799,17 +4729,16 @@
       <c r="A114">
         <v>113</v>
       </c>
-      <c r="B114" s="12" t="s">
+      <c r="B114" t="s">
         <v>150</v>
       </c>
-      <c r="C114" s="12" t="s">
+      <c r="C114" t="s">
         <v>142</v>
       </c>
-      <c r="D114" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12" t="s">
+      <c r="D114" t="s">
+        <v>34</v>
+      </c>
+      <c r="F114" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4817,17 +4746,16 @@
       <c r="A115">
         <v>114</v>
       </c>
-      <c r="B115" s="12" t="s">
+      <c r="B115" t="s">
         <v>259</v>
       </c>
-      <c r="C115" s="12" t="s">
+      <c r="C115" t="s">
         <v>142</v>
       </c>
-      <c r="D115" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E115" s="12"/>
-      <c r="F115" s="12" t="s">
+      <c r="D115" t="s">
+        <v>34</v>
+      </c>
+      <c r="F115" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4835,197 +4763,196 @@
       <c r="A116">
         <v>115</v>
       </c>
-      <c r="B116" s="12" t="s">
+      <c r="B116" t="s">
         <v>260</v>
       </c>
-      <c r="C116" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D116" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C116" t="s">
+        <v>33</v>
+      </c>
+      <c r="D116" t="s">
+        <v>34</v>
+      </c>
+      <c r="F116" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>117</v>
       </c>
-      <c r="B117" s="12" t="s">
+      <c r="B117" t="s">
         <v>263</v>
       </c>
-      <c r="C117" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D117" s="12" t="s">
+      <c r="C117" t="s">
+        <v>33</v>
+      </c>
+      <c r="D117" t="s">
         <v>10</v>
       </c>
-      <c r="E117" s="12" t="s">
+      <c r="E117" t="s">
         <v>325</v>
       </c>
-      <c r="F117" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F117" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>118</v>
       </c>
-      <c r="B118" s="12" t="s">
+      <c r="B118" t="s">
         <v>264</v>
       </c>
-      <c r="C118" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D118" s="12" t="s">
+      <c r="C118" t="s">
+        <v>33</v>
+      </c>
+      <c r="D118" t="s">
         <v>11</v>
       </c>
-      <c r="E118" s="12" t="s">
+      <c r="E118" t="s">
         <v>325</v>
       </c>
-      <c r="F118" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F118" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>139</v>
       </c>
-      <c r="B119" s="12" t="s">
+      <c r="B119" t="s">
         <v>287</v>
       </c>
-      <c r="C119" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D119" s="12" t="s">
+      <c r="C119" t="s">
+        <v>33</v>
+      </c>
+      <c r="D119" t="s">
         <v>12</v>
       </c>
-      <c r="E119" s="12" t="s">
+      <c r="E119" t="s">
         <v>325</v>
       </c>
-      <c r="F119" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F119" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>140</v>
       </c>
-      <c r="B120" s="12" t="s">
+      <c r="B120" t="s">
         <v>288</v>
       </c>
-      <c r="C120" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D120" s="12" t="s">
+      <c r="C120" t="s">
+        <v>33</v>
+      </c>
+      <c r="D120" t="s">
         <v>13</v>
       </c>
-      <c r="E120" s="12" t="s">
+      <c r="E120" t="s">
         <v>325</v>
       </c>
-      <c r="F120" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F120" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>141</v>
       </c>
-      <c r="B121" s="12" t="s">
+      <c r="B121" t="s">
         <v>289</v>
       </c>
-      <c r="C121" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D121" s="12" t="s">
+      <c r="C121" t="s">
+        <v>33</v>
+      </c>
+      <c r="D121" t="s">
         <v>290</v>
       </c>
-      <c r="E121" s="12" t="s">
+      <c r="E121" t="s">
         <v>325</v>
       </c>
-      <c r="F121" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F121" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>144</v>
       </c>
-      <c r="B122" s="12" t="s">
+      <c r="B122" t="s">
         <v>293</v>
       </c>
-      <c r="C122" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D122" s="12" t="s">
+      <c r="C122" t="s">
+        <v>33</v>
+      </c>
+      <c r="D122" t="s">
         <v>9</v>
       </c>
-      <c r="E122" s="12" t="s">
+      <c r="E122" t="s">
         <v>325</v>
       </c>
-      <c r="F122" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F122" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>33</v>
       </c>
-      <c r="B123" s="12" t="s">
+      <c r="B123" t="s">
         <v>172</v>
       </c>
-      <c r="C123" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D123" s="12" t="s">
+      <c r="C123" t="s">
+        <v>33</v>
+      </c>
+      <c r="D123" t="s">
         <v>20</v>
       </c>
-      <c r="E123" s="12" t="s">
+      <c r="E123" t="s">
         <v>4</v>
       </c>
-      <c r="F123" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F123" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>34</v>
       </c>
-      <c r="B124" s="12" t="s">
+      <c r="B124" t="s">
         <v>173</v>
       </c>
-      <c r="C124" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D124" s="12" t="s">
+      <c r="C124" t="s">
+        <v>33</v>
+      </c>
+      <c r="D124" t="s">
         <v>19</v>
       </c>
-      <c r="E124" s="12" t="s">
+      <c r="E124" t="s">
         <v>4</v>
       </c>
-      <c r="F124" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F124" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>93</v>
       </c>
-      <c r="B125" s="12" t="s">
+      <c r="B125" t="s">
         <v>238</v>
       </c>
-      <c r="C125" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D125" s="12" t="s">
+      <c r="C125" t="s">
+        <v>33</v>
+      </c>
+      <c r="D125" t="s">
         <v>18</v>
       </c>
-      <c r="E125" s="12" t="s">
+      <c r="E125" t="s">
         <v>4</v>
       </c>
-      <c r="F125" s="12" t="s">
+      <c r="F125" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5033,17 +4960,16 @@
       <c r="A126">
         <v>125</v>
       </c>
-      <c r="B126" s="12" t="s">
+      <c r="B126" t="s">
         <v>229</v>
       </c>
-      <c r="C126" s="12" t="s">
+      <c r="C126" t="s">
         <v>142</v>
       </c>
-      <c r="D126" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E126" s="12"/>
-      <c r="F126" s="12" t="s">
+      <c r="D126" t="s">
+        <v>34</v>
+      </c>
+      <c r="F126" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5051,17 +4977,16 @@
       <c r="A127">
         <v>126</v>
       </c>
-      <c r="B127" s="12" t="s">
+      <c r="B127" t="s">
         <v>150</v>
       </c>
-      <c r="C127" s="12" t="s">
+      <c r="C127" t="s">
         <v>142</v>
       </c>
-      <c r="D127" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E127" s="12"/>
-      <c r="F127" s="12" t="s">
+      <c r="D127" t="s">
+        <v>34</v>
+      </c>
+      <c r="F127" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5069,17 +4994,16 @@
       <c r="A128">
         <v>127</v>
       </c>
-      <c r="B128" s="12" t="s">
+      <c r="B128" t="s">
         <v>151</v>
       </c>
-      <c r="C128" s="12" t="s">
+      <c r="C128" t="s">
         <v>142</v>
       </c>
-      <c r="D128" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E128" s="12"/>
-      <c r="F128" s="12" t="s">
+      <c r="D128" t="s">
+        <v>34</v>
+      </c>
+      <c r="F128" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5087,17 +5011,16 @@
       <c r="A129">
         <v>128</v>
       </c>
-      <c r="B129" s="12" t="s">
+      <c r="B129" t="s">
         <v>277</v>
       </c>
-      <c r="C129" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D129" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E129" s="12"/>
-      <c r="F129" s="12" t="s">
+      <c r="C129" t="s">
+        <v>33</v>
+      </c>
+      <c r="D129" t="s">
+        <v>34</v>
+      </c>
+      <c r="F129" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5105,17 +5028,16 @@
       <c r="A130">
         <v>129</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="B130" t="s">
         <v>278</v>
       </c>
-      <c r="C130" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D130" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E130" s="12"/>
-      <c r="F130" s="12" t="s">
+      <c r="C130" t="s">
+        <v>33</v>
+      </c>
+      <c r="D130" t="s">
+        <v>34</v>
+      </c>
+      <c r="F130" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5123,17 +5045,16 @@
       <c r="A131">
         <v>130</v>
       </c>
-      <c r="B131" s="12" t="s">
+      <c r="B131" t="s">
         <v>279</v>
       </c>
-      <c r="C131" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D131" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E131" s="12"/>
-      <c r="F131" s="12" t="s">
+      <c r="C131" t="s">
+        <v>33</v>
+      </c>
+      <c r="D131" t="s">
+        <v>34</v>
+      </c>
+      <c r="F131" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5141,17 +5062,16 @@
       <c r="A132">
         <v>131</v>
       </c>
-      <c r="B132" s="12" t="s">
+      <c r="B132" t="s">
         <v>280</v>
       </c>
-      <c r="C132" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D132" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E132" s="12"/>
-      <c r="F132" s="12" t="s">
+      <c r="C132" t="s">
+        <v>33</v>
+      </c>
+      <c r="D132" t="s">
+        <v>34</v>
+      </c>
+      <c r="F132" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5159,17 +5079,16 @@
       <c r="A133">
         <v>132</v>
       </c>
-      <c r="B133" s="12" t="s">
+      <c r="B133" t="s">
         <v>281</v>
       </c>
-      <c r="C133" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D133" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E133" s="12"/>
-      <c r="F133" s="12" t="s">
+      <c r="C133" t="s">
+        <v>33</v>
+      </c>
+      <c r="D133" t="s">
+        <v>34</v>
+      </c>
+      <c r="F133" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5177,17 +5096,16 @@
       <c r="A134">
         <v>133</v>
       </c>
-      <c r="B134" s="12" t="s">
+      <c r="B134" t="s">
         <v>282</v>
       </c>
-      <c r="C134" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D134" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12" t="s">
+      <c r="C134" t="s">
+        <v>33</v>
+      </c>
+      <c r="D134" t="s">
+        <v>34</v>
+      </c>
+      <c r="F134" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5195,17 +5113,16 @@
       <c r="A135">
         <v>134</v>
       </c>
-      <c r="B135" s="12" t="s">
+      <c r="B135" t="s">
         <v>283</v>
       </c>
-      <c r="C135" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D135" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E135" s="12"/>
-      <c r="F135" s="12" t="s">
+      <c r="C135" t="s">
+        <v>33</v>
+      </c>
+      <c r="D135" t="s">
+        <v>34</v>
+      </c>
+      <c r="F135" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5213,17 +5130,16 @@
       <c r="A136">
         <v>135</v>
       </c>
-      <c r="B136" s="12" t="s">
+      <c r="B136" t="s">
         <v>150</v>
       </c>
-      <c r="C136" s="12" t="s">
+      <c r="C136" t="s">
         <v>142</v>
       </c>
-      <c r="D136" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E136" s="12"/>
-      <c r="F136" s="12" t="s">
+      <c r="D136" t="s">
+        <v>34</v>
+      </c>
+      <c r="F136" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5231,37 +5147,36 @@
       <c r="A137">
         <v>136</v>
       </c>
-      <c r="B137" s="12" t="s">
+      <c r="B137" t="s">
         <v>151</v>
       </c>
-      <c r="C137" s="12" t="s">
+      <c r="C137" t="s">
         <v>142</v>
       </c>
-      <c r="D137" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E137" s="12"/>
-      <c r="F137" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D137" t="s">
+        <v>34</v>
+      </c>
+      <c r="F137" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>116</v>
       </c>
-      <c r="B138" s="12" t="s">
+      <c r="B138" t="s">
         <v>261</v>
       </c>
-      <c r="C138" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D138" s="12" t="s">
+      <c r="C138" t="s">
+        <v>33</v>
+      </c>
+      <c r="D138" t="s">
         <v>262</v>
       </c>
-      <c r="E138" s="12" t="s">
+      <c r="E138" t="s">
         <v>8</v>
       </c>
-      <c r="F138" s="12" t="s">
+      <c r="F138" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5269,77 +5184,76 @@
       <c r="A139">
         <v>138</v>
       </c>
-      <c r="B139" s="12" t="s">
+      <c r="B139" t="s">
         <v>286</v>
       </c>
-      <c r="C139" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D139" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E139" s="12"/>
-      <c r="F139" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C139" t="s">
+        <v>33</v>
+      </c>
+      <c r="D139" t="s">
+        <v>34</v>
+      </c>
+      <c r="F139" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>124</v>
       </c>
-      <c r="B140" s="12" t="s">
+      <c r="B140" t="s">
         <v>275</v>
       </c>
-      <c r="C140" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D140" s="12" t="s">
+      <c r="C140" t="s">
+        <v>33</v>
+      </c>
+      <c r="D140" t="s">
         <v>276</v>
       </c>
-      <c r="E140" s="12" t="s">
+      <c r="E140" t="s">
         <v>8</v>
       </c>
-      <c r="F140" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F140" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>137</v>
       </c>
-      <c r="B141" s="12" t="s">
+      <c r="B141" t="s">
         <v>284</v>
       </c>
-      <c r="C141" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D141" s="12" t="s">
+      <c r="C141" t="s">
+        <v>33</v>
+      </c>
+      <c r="D141" t="s">
         <v>285</v>
       </c>
-      <c r="E141" s="12" t="s">
+      <c r="E141" t="s">
         <v>8</v>
       </c>
-      <c r="F141" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F141" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>119</v>
       </c>
-      <c r="B142" s="12" t="s">
+      <c r="B142" t="s">
         <v>265</v>
       </c>
-      <c r="C142" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D142" s="12" t="s">
+      <c r="C142" t="s">
+        <v>33</v>
+      </c>
+      <c r="D142" t="s">
         <v>266</v>
       </c>
-      <c r="E142" s="12" t="s">
+      <c r="E142" t="s">
         <v>111</v>
       </c>
-      <c r="F142" s="12" t="s">
+      <c r="F142" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5347,17 +5261,16 @@
       <c r="A143">
         <v>142</v>
       </c>
-      <c r="B143" s="12" t="s">
+      <c r="B143" t="s">
         <v>291</v>
       </c>
-      <c r="C143" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D143" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E143" s="12"/>
-      <c r="F143" s="12" t="s">
+      <c r="C143" t="s">
+        <v>33</v>
+      </c>
+      <c r="D143" t="s">
+        <v>34</v>
+      </c>
+      <c r="F143" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5365,37 +5278,36 @@
       <c r="A144">
         <v>143</v>
       </c>
-      <c r="B144" s="12" t="s">
+      <c r="B144" t="s">
         <v>292</v>
       </c>
-      <c r="C144" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D144" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E144" s="12"/>
-      <c r="F144" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C144" t="s">
+        <v>33</v>
+      </c>
+      <c r="D144" t="s">
+        <v>34</v>
+      </c>
+      <c r="F144" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>120</v>
       </c>
-      <c r="B145" s="12" t="s">
+      <c r="B145" t="s">
         <v>267</v>
       </c>
-      <c r="C145" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D145" s="12" t="s">
+      <c r="C145" t="s">
+        <v>33</v>
+      </c>
+      <c r="D145" t="s">
         <v>268</v>
       </c>
-      <c r="E145" s="12" t="s">
+      <c r="E145" t="s">
         <v>111</v>
       </c>
-      <c r="F145" s="12" t="s">
+      <c r="F145" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5403,17 +5315,16 @@
       <c r="A146">
         <v>145</v>
       </c>
-      <c r="B146" s="12" t="s">
+      <c r="B146" t="s">
         <v>294</v>
       </c>
-      <c r="C146" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D146" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E146" s="12"/>
-      <c r="F146" s="12" t="s">
+      <c r="C146" t="s">
+        <v>33</v>
+      </c>
+      <c r="D146" t="s">
+        <v>34</v>
+      </c>
+      <c r="F146" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5421,17 +5332,16 @@
       <c r="A147">
         <v>146</v>
       </c>
-      <c r="B147" s="12" t="s">
+      <c r="B147" t="s">
         <v>295</v>
       </c>
-      <c r="C147" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D147" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E147" s="12"/>
-      <c r="F147" s="12" t="s">
+      <c r="C147" t="s">
+        <v>33</v>
+      </c>
+      <c r="D147" t="s">
+        <v>34</v>
+      </c>
+      <c r="F147" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5439,17 +5349,16 @@
       <c r="A148">
         <v>147</v>
       </c>
-      <c r="B148" s="12" t="s">
+      <c r="B148" t="s">
         <v>296</v>
       </c>
-      <c r="C148" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D148" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E148" s="12"/>
-      <c r="F148" s="12" t="s">
+      <c r="C148" t="s">
+        <v>33</v>
+      </c>
+      <c r="D148" t="s">
+        <v>34</v>
+      </c>
+      <c r="F148" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5457,17 +5366,16 @@
       <c r="A149">
         <v>148</v>
       </c>
-      <c r="B149" s="12" t="s">
+      <c r="B149" t="s">
         <v>150</v>
       </c>
-      <c r="C149" s="12" t="s">
+      <c r="C149" t="s">
         <v>142</v>
       </c>
-      <c r="D149" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E149" s="12"/>
-      <c r="F149" s="12" t="s">
+      <c r="D149" t="s">
+        <v>34</v>
+      </c>
+      <c r="F149" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5475,17 +5383,16 @@
       <c r="A150">
         <v>149</v>
       </c>
-      <c r="B150" s="12" t="s">
+      <c r="B150" t="s">
         <v>151</v>
       </c>
-      <c r="C150" s="12" t="s">
+      <c r="C150" t="s">
         <v>142</v>
       </c>
-      <c r="D150" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E150" s="12"/>
-      <c r="F150" s="12" t="s">
+      <c r="D150" t="s">
+        <v>34</v>
+      </c>
+      <c r="F150" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5493,17 +5400,16 @@
       <c r="A151">
         <v>150</v>
       </c>
-      <c r="B151" s="12" t="s">
+      <c r="B151" t="s">
         <v>297</v>
       </c>
-      <c r="C151" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D151" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E151" s="12"/>
-      <c r="F151" s="12" t="s">
+      <c r="C151" t="s">
+        <v>33</v>
+      </c>
+      <c r="D151" t="s">
+        <v>34</v>
+      </c>
+      <c r="F151" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5511,17 +5417,16 @@
       <c r="A152">
         <v>151</v>
       </c>
-      <c r="B152" s="12" t="s">
+      <c r="B152" t="s">
         <v>298</v>
       </c>
-      <c r="C152" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D152" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E152" s="12"/>
-      <c r="F152" s="12" t="s">
+      <c r="C152" t="s">
+        <v>33</v>
+      </c>
+      <c r="D152" t="s">
+        <v>34</v>
+      </c>
+      <c r="F152" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5529,17 +5434,16 @@
       <c r="A153">
         <v>152</v>
       </c>
-      <c r="B153" s="12" t="s">
+      <c r="B153" t="s">
         <v>299</v>
       </c>
-      <c r="C153" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D153" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E153" s="12"/>
-      <c r="F153" s="12" t="s">
+      <c r="C153" t="s">
+        <v>33</v>
+      </c>
+      <c r="D153" t="s">
+        <v>34</v>
+      </c>
+      <c r="F153" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5547,17 +5451,16 @@
       <c r="A154">
         <v>153</v>
       </c>
-      <c r="B154" s="12" t="s">
+      <c r="B154" t="s">
         <v>300</v>
       </c>
-      <c r="C154" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D154" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E154" s="12"/>
-      <c r="F154" s="12" t="s">
+      <c r="C154" t="s">
+        <v>33</v>
+      </c>
+      <c r="D154" t="s">
+        <v>34</v>
+      </c>
+      <c r="F154" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5565,17 +5468,16 @@
       <c r="A155">
         <v>154</v>
       </c>
-      <c r="B155" s="12" t="s">
+      <c r="B155" t="s">
         <v>301</v>
       </c>
-      <c r="C155" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D155" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E155" s="12"/>
-      <c r="F155" s="12" t="s">
+      <c r="C155" t="s">
+        <v>33</v>
+      </c>
+      <c r="D155" t="s">
+        <v>34</v>
+      </c>
+      <c r="F155" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5583,17 +5485,16 @@
       <c r="A156">
         <v>155</v>
       </c>
-      <c r="B156" s="12" t="s">
+      <c r="B156" t="s">
         <v>302</v>
       </c>
-      <c r="C156" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D156" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E156" s="12"/>
-      <c r="F156" s="12" t="s">
+      <c r="C156" t="s">
+        <v>33</v>
+      </c>
+      <c r="D156" t="s">
+        <v>34</v>
+      </c>
+      <c r="F156" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5601,17 +5502,16 @@
       <c r="A157">
         <v>156</v>
       </c>
-      <c r="B157" s="12" t="s">
+      <c r="B157" t="s">
         <v>303</v>
       </c>
-      <c r="C157" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D157" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E157" s="12"/>
-      <c r="F157" s="12" t="s">
+      <c r="C157" t="s">
+        <v>33</v>
+      </c>
+      <c r="D157" t="s">
+        <v>34</v>
+      </c>
+      <c r="F157" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5619,17 +5519,16 @@
       <c r="A158">
         <v>157</v>
       </c>
-      <c r="B158" s="12" t="s">
+      <c r="B158" t="s">
         <v>304</v>
       </c>
-      <c r="C158" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D158" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E158" s="12"/>
-      <c r="F158" s="12" t="s">
+      <c r="C158" t="s">
+        <v>33</v>
+      </c>
+      <c r="D158" t="s">
+        <v>34</v>
+      </c>
+      <c r="F158" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5637,17 +5536,16 @@
       <c r="A159">
         <v>158</v>
       </c>
-      <c r="B159" s="12" t="s">
+      <c r="B159" t="s">
         <v>150</v>
       </c>
-      <c r="C159" s="12" t="s">
+      <c r="C159" t="s">
         <v>142</v>
       </c>
-      <c r="D159" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E159" s="12"/>
-      <c r="F159" s="12" t="s">
+      <c r="D159" t="s">
+        <v>34</v>
+      </c>
+      <c r="F159" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5655,17 +5553,16 @@
       <c r="A160">
         <v>159</v>
       </c>
-      <c r="B160" s="12" t="s">
+      <c r="B160" t="s">
         <v>151</v>
       </c>
-      <c r="C160" s="12" t="s">
+      <c r="C160" t="s">
         <v>142</v>
       </c>
-      <c r="D160" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E160" s="12"/>
-      <c r="F160" s="12" t="s">
+      <c r="D160" t="s">
+        <v>34</v>
+      </c>
+      <c r="F160" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5673,17 +5570,16 @@
       <c r="A161">
         <v>160</v>
       </c>
-      <c r="B161" s="12" t="s">
+      <c r="B161" t="s">
         <v>305</v>
       </c>
-      <c r="C161" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D161" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E161" s="12"/>
-      <c r="F161" s="12" t="s">
+      <c r="C161" t="s">
+        <v>33</v>
+      </c>
+      <c r="D161" t="s">
+        <v>34</v>
+      </c>
+      <c r="F161" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5691,17 +5587,16 @@
       <c r="A162">
         <v>161</v>
       </c>
-      <c r="B162" s="12" t="s">
+      <c r="B162" t="s">
         <v>306</v>
       </c>
-      <c r="C162" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D162" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E162" s="12"/>
-      <c r="F162" s="12" t="s">
+      <c r="C162" t="s">
+        <v>33</v>
+      </c>
+      <c r="D162" t="s">
+        <v>34</v>
+      </c>
+      <c r="F162" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5709,17 +5604,16 @@
       <c r="A163">
         <v>162</v>
       </c>
-      <c r="B163" s="12" t="s">
+      <c r="B163" t="s">
         <v>307</v>
       </c>
-      <c r="C163" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D163" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E163" s="12"/>
-      <c r="F163" s="12" t="s">
+      <c r="C163" t="s">
+        <v>33</v>
+      </c>
+      <c r="D163" t="s">
+        <v>34</v>
+      </c>
+      <c r="F163" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5727,57 +5621,56 @@
       <c r="A164">
         <v>163</v>
       </c>
-      <c r="B164" s="12" t="s">
+      <c r="B164" t="s">
         <v>308</v>
       </c>
-      <c r="C164" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D164" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E164" s="12"/>
-      <c r="F164" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C164" t="s">
+        <v>33</v>
+      </c>
+      <c r="D164" t="s">
+        <v>34</v>
+      </c>
+      <c r="F164" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>121</v>
       </c>
-      <c r="B165" s="12" t="s">
+      <c r="B165" t="s">
         <v>269</v>
       </c>
-      <c r="C165" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D165" s="12" t="s">
+      <c r="C165" t="s">
+        <v>33</v>
+      </c>
+      <c r="D165" t="s">
         <v>270</v>
       </c>
-      <c r="E165" s="12" t="s">
+      <c r="E165" t="s">
         <v>111</v>
       </c>
-      <c r="F165" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F165" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>122</v>
       </c>
-      <c r="B166" s="12" t="s">
+      <c r="B166" t="s">
         <v>271</v>
       </c>
-      <c r="C166" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D166" s="12" t="s">
+      <c r="C166" t="s">
+        <v>33</v>
+      </c>
+      <c r="D166" t="s">
         <v>272</v>
       </c>
-      <c r="E166" s="12" t="s">
+      <c r="E166" t="s">
         <v>111</v>
       </c>
-      <c r="F166" s="12" t="s">
+      <c r="F166" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5785,17 +5678,16 @@
       <c r="A167">
         <v>166</v>
       </c>
-      <c r="B167" s="12" t="s">
+      <c r="B167" t="s">
         <v>311</v>
       </c>
-      <c r="C167" s="12" t="s">
+      <c r="C167" t="s">
         <v>312</v>
       </c>
-      <c r="D167" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E167" s="12"/>
-      <c r="F167" s="12" t="s">
+      <c r="D167" t="s">
+        <v>34</v>
+      </c>
+      <c r="F167" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5803,17 +5695,16 @@
       <c r="A168">
         <v>167</v>
       </c>
-      <c r="B168" s="12" t="s">
+      <c r="B168" t="s">
         <v>313</v>
       </c>
-      <c r="C168" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D168" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E168" s="12"/>
-      <c r="F168" s="12" t="s">
+      <c r="C168" t="s">
+        <v>33</v>
+      </c>
+      <c r="D168" t="s">
+        <v>34</v>
+      </c>
+      <c r="F168" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5821,37 +5712,36 @@
       <c r="A169">
         <v>168</v>
       </c>
-      <c r="B169" s="12" t="s">
+      <c r="B169" t="s">
         <v>314</v>
       </c>
-      <c r="C169" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D169" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E169" s="12"/>
-      <c r="F169" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C169" t="s">
+        <v>33</v>
+      </c>
+      <c r="D169" t="s">
+        <v>34</v>
+      </c>
+      <c r="F169" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>123</v>
       </c>
-      <c r="B170" s="12" t="s">
+      <c r="B170" t="s">
         <v>273</v>
       </c>
-      <c r="C170" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D170" s="12" t="s">
+      <c r="C170" t="s">
+        <v>33</v>
+      </c>
+      <c r="D170" t="s">
         <v>274</v>
       </c>
-      <c r="E170" s="12" t="s">
+      <c r="E170" t="s">
         <v>111</v>
       </c>
-      <c r="F170" s="12" t="s">
+      <c r="F170" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5859,17 +5749,16 @@
       <c r="A171">
         <v>170</v>
       </c>
-      <c r="B171" s="12" t="s">
+      <c r="B171" t="s">
         <v>317</v>
       </c>
-      <c r="C171" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D171" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E171" s="12"/>
-      <c r="F171" s="12" t="s">
+      <c r="C171" t="s">
+        <v>33</v>
+      </c>
+      <c r="D171" t="s">
+        <v>34</v>
+      </c>
+      <c r="F171" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5877,17 +5766,16 @@
       <c r="A172">
         <v>171</v>
       </c>
-      <c r="B172" s="12" t="s">
+      <c r="B172" t="s">
         <v>318</v>
       </c>
-      <c r="C172" s="12" t="s">
+      <c r="C172" t="s">
         <v>142</v>
       </c>
-      <c r="D172" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E172" s="12"/>
-      <c r="F172" s="12" t="s">
+      <c r="D172" t="s">
+        <v>34</v>
+      </c>
+      <c r="F172" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5895,17 +5783,16 @@
       <c r="A173">
         <v>172</v>
       </c>
-      <c r="B173" s="12" t="s">
+      <c r="B173" t="s">
         <v>151</v>
       </c>
-      <c r="C173" s="12" t="s">
+      <c r="C173" t="s">
         <v>142</v>
       </c>
-      <c r="D173" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E173" s="12"/>
-      <c r="F173" s="12" t="s">
+      <c r="D173" t="s">
+        <v>34</v>
+      </c>
+      <c r="F173" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5913,17 +5800,16 @@
       <c r="A174">
         <v>173</v>
       </c>
-      <c r="B174" s="12" t="s">
+      <c r="B174" t="s">
         <v>319</v>
       </c>
-      <c r="C174" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D174" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E174" s="12"/>
-      <c r="F174" s="12" t="s">
+      <c r="C174" t="s">
+        <v>33</v>
+      </c>
+      <c r="D174" t="s">
+        <v>34</v>
+      </c>
+      <c r="F174" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5931,17 +5817,16 @@
       <c r="A175">
         <v>174</v>
       </c>
-      <c r="B175" s="12" t="s">
+      <c r="B175" t="s">
         <v>320</v>
       </c>
-      <c r="C175" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D175" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E175" s="12"/>
-      <c r="F175" s="12" t="s">
+      <c r="C175" t="s">
+        <v>33</v>
+      </c>
+      <c r="D175" t="s">
+        <v>34</v>
+      </c>
+      <c r="F175" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5949,17 +5834,16 @@
       <c r="A176">
         <v>175</v>
       </c>
-      <c r="B176" s="12" t="s">
+      <c r="B176" t="s">
         <v>321</v>
       </c>
-      <c r="C176" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D176" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E176" s="12"/>
-      <c r="F176" s="12" t="s">
+      <c r="C176" t="s">
+        <v>33</v>
+      </c>
+      <c r="D176" t="s">
+        <v>34</v>
+      </c>
+      <c r="F176" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5967,17 +5851,16 @@
       <c r="A177">
         <v>176</v>
       </c>
-      <c r="B177" s="12" t="s">
+      <c r="B177" t="s">
         <v>322</v>
       </c>
-      <c r="C177" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D177" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E177" s="12"/>
-      <c r="F177" s="12" t="s">
+      <c r="C177" t="s">
+        <v>33</v>
+      </c>
+      <c r="D177" t="s">
+        <v>34</v>
+      </c>
+      <c r="F177" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>